<commit_message>
adding new power and imc_access capabilities.
</commit_message>
<xml_diff>
--- a/Settings.xlsx
+++ b/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tyscott\scotttyso\intersight_iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDDD7C3-C9A6-444F-85E9-0F33854FAD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597B4A84-6846-4FEC-A251-50D11E30B0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="803" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4433,8 +4433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A250C3-9683-4B6C-B4E9-67AA5B03538C}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R43" sqref="R43:R47"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>